<commit_message>
parser not working properly
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
   <si>
     <t>Question</t>
   </si>
@@ -36,6 +36,27 @@
   </si>
   <si>
     <t>Correct Answer</t>
+  </si>
+  <si>
+    <t>this is question 1 ? A.this is A option for q1. B.this is B option for q1. C.this is C option for q1. D.and this is D option for q1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>this is question 2 ? A.this is A option for q2. B.this is B option for q2. C.this is C option for q2. D.and this is D option for q2.</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>this is question 3 ? A.this is A option for q3. B.this is B option for q3. C.this is C option for q3. D.and this is D option for q3.</t>
+  </si>
+  <si>
+    <t>this is question 4 ? A.this is A option for q4. B.this is B option for q4. C.this is C option for q4. D.and this is D option for q4.</t>
   </si>
 </sst>
 </file>
@@ -80,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -112,6 +133,110 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>